<commit_message>
Correção e atualização 13/11
</commit_message>
<xml_diff>
--- a/PVs/laje.xlsx
+++ b/PVs/laje.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonardo.leao\Desktop\Concrete-Instrum-Scripts\PVs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\Iniciação Científica\Instrumentação do concreto\Concrete-Instrum-Scripts\PVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AD3835-AEB8-41CC-9D84-8B7EA2C93918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0D0905-BBC3-4FC9-AC06-C5E79AD013DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1785" windowWidth="21600" windowHeight="11400" xr2:uid="{D1ED5E16-0395-4A7E-9D10-013CF81259EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D1ED5E16-0395-4A7E-9D10-013CF81259EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>Localização</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>L16</t>
+  </si>
+  <si>
+    <t>L2L3</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F66DE42E-832C-49A5-B01B-44813F8C9F48}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,353 +526,441 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D16" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2">
         <v>10</v>
-      </c>
-      <c r="C18" s="3">
-        <v>20</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C21" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3">
         <v>18</v>
       </c>
       <c r="D24" s="2">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25" s="3">
         <v>18</v>
       </c>
       <c r="D25" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C27" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28" s="3">
         <v>20</v>
       </c>
       <c r="D28" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="3">
         <v>20</v>
       </c>
       <c r="D29" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3">
+        <v>20</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="3">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3">
+        <v>20</v>
+      </c>
+      <c r="D37" s="2">
         <v>12</v>
       </c>
     </row>

</xml_diff>